<commit_message>
chaz version of schedule
</commit_message>
<xml_diff>
--- a/Shared Documentation/Luke's Documents/Clash of Cosplayers - Deliverables.xlsx
+++ b/Shared Documentation/Luke's Documents/Clash of Cosplayers - Deliverables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C2240950\Documents\GitHub\Project_Clash-of-Cosplayers\Shared Documentation\Luke's Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7D36F7-E190-47BF-B4F3-FDDC6E98156B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E01BFA-5C37-496B-948F-DB65C74466AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{E57F7292-3F36-47CF-B64B-390F0A8E2C94}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{E57F7292-3F36-47CF-B64B-390F0A8E2C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Asset name</t>
   </si>
@@ -59,15 +59,6 @@
     <t>Trolley</t>
   </si>
   <si>
-    <t>Taser [stun]</t>
-  </si>
-  <si>
-    <t>Water [glass]</t>
-  </si>
-  <si>
-    <t>Lighter [flame]</t>
-  </si>
-  <si>
     <t>oil flask (extra)</t>
   </si>
   <si>
@@ -123,6 +114,33 @@
   </si>
   <si>
     <t>Equipment</t>
+  </si>
+  <si>
+    <t>Enemies:</t>
+  </si>
+  <si>
+    <t>Basic Contestant</t>
+  </si>
+  <si>
+    <t>Zues (Extra)</t>
+  </si>
+  <si>
+    <t>boss</t>
+  </si>
+  <si>
+    <t>reward from "Zues"</t>
+  </si>
+  <si>
+    <t>Lighter [flame] (extra)</t>
+  </si>
+  <si>
+    <t>Water [glass] (extra)</t>
+  </si>
+  <si>
+    <t>Taser [stun] (extra)</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -516,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BD4154-D683-48E3-B727-AD028CFBFA14}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E9" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
   </cols>
@@ -558,116 +576,149 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>